<commit_message>
Syntax checking stable and moved to new filing system, initial draft of consistency checking
</commit_message>
<xml_diff>
--- a/AEF_files/10.syntax.passed/202504251541---Thailand AEF_2023.syntax_checked.xlsx
+++ b/AEF_files/10.syntax.passed/202504251541---Thailand AEF_2023.syntax_checked.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="7080" yWindow="9800" windowWidth="38460" windowHeight="17720" tabRatio="618" firstSheet="0" activeTab="4" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="7080" yWindow="9800" windowWidth="38460" windowHeight="17720" tabRatio="618" firstSheet="0" activeTab="2" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Index" sheetId="1" state="visible" r:id="rId1"/>
@@ -2269,8 +2269,8 @@
   </sheetPr>
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScale="216" zoomScaleNormal="139" zoomScaleSheetLayoutView="216" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="216" zoomScaleNormal="139" zoomScaleSheetLayoutView="216" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -2301,7 +2301,7 @@
       </c>
       <c r="C4" s="8" t="inlineStr">
         <is>
-          <t>TH</t>
+          <t>THA</t>
         </is>
       </c>
     </row>
@@ -2840,7 +2840,7 @@
   </sheetPr>
   <dimension ref="A1:AH11"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="90" zoomScaleNormal="74" zoomScaleSheetLayoutView="90" workbookViewId="0">
+    <sheetView view="pageBreakPreview" zoomScale="90" zoomScaleNormal="74" zoomScaleSheetLayoutView="90" workbookViewId="0">
       <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
@@ -4771,8 +4771,8 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008FB6730B0802B54A9F00C78B857E1443" ma:contentTypeVersion="21" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e7d0671dbe340d15fdce5ab7e9f4c491">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="819ae873-75e1-413b-9d00-7af9258cf281" xmlns:ns3="eb4559c4-8463-4985-927f-f0d558bff8f0" xmlns:ns4="13d80b15-5f07-43ab-b435-85767a7dac08" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2feafd61044eb4abe44eb47c2e62f3e5" ns2:_="" ns3:_="" ns4:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008FB6730B0802B54A9F00C78B857E1443" ma:contentTypeVersion="21" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e758502e7902c92bdb050e89a8fea950">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="819ae873-75e1-413b-9d00-7af9258cf281" xmlns:ns3="eb4559c4-8463-4985-927f-f0d558bff8f0" xmlns:ns4="13d80b15-5f07-43ab-b435-85767a7dac08" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f4060acd4b29e25a8a76462245842ebf" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="819ae873-75e1-413b-9d00-7af9258cf281"/>
     <xsd:import namespace="eb4559c4-8463-4985-927f-f0d558bff8f0"/>
     <xsd:import namespace="13d80b15-5f07-43ab-b435-85767a7dac08"/>
@@ -5082,17 +5082,17 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5C0E5C32-557C-4376-A148-90DDD395863A}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0E1FDC6E-B636-4FE0-B398-EB528D8067CE}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9FDE34E6-F405-47FD-81AA-B14D4F530AAF}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F42C5F8D-22AC-4286-AD4C-EAD0C1C5E66C}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DD75082D-1A5C-4F92-B9BA-4AC8227B1571}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A9799D65-07E5-48E8-AA39-49E0191F739B}"/>
 </file>
 
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9E7A1DC0-3593-43F8-8CA7-8DAB8858379E}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F09D9509-AE1F-4384-AA74-2A606E86234E}"/>
 </file>
</xml_diff>